<commit_message>
Created Main Class for SPDU and slightly modified the table
</commit_message>
<xml_diff>
--- a/SPDU/SPDU Parameters.xlsx
+++ b/SPDU/SPDU Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\othow\PycharmProjects\ccsds-sc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\othow\PycharmProjects\ccsds-sc2\SPDU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A75E2B9-9E03-41A4-9389-7A4756A678C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EF726D-04DD-495C-AF82-484E3383C3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B05163AC-0A20-4B63-99D4-7D5E74A884FE}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="19420" windowHeight="11500" xr2:uid="{B05163AC-0A20-4B63-99D4-7D5E74A884FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,6 +512,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -521,45 +560,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,19 +886,19 @@
   </sheetPr>
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D24"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
     <col min="3" max="3" width="24.26953125" customWidth="1"/>
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -925,21 +925,21 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="48"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
@@ -958,7 +958,7 @@
       <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -974,12 +974,12 @@
       <c r="F3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -989,11 +989,11 @@
       <c r="E4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1011,7 +1011,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1032,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="19"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19"/>
+      <c r="A8" s="48"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1089,7 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1126,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="19"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="19"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1196,14 +1196,14 @@
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="19"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="37"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="13" t="s">
         <v>48</v>
       </c>
@@ -1215,14 +1215,14 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="19"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="13" t="s">
         <v>44</v>
       </c>
@@ -1234,224 +1234,224 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="19"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="35" t="s">
+      <c r="D18" s="32"/>
+      <c r="E18" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="49"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="19"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="29" t="s">
+      <c r="D19" s="32"/>
+      <c r="E19" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="19"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="35"/>
+      <c r="E20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="19"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="23" t="s">
+      <c r="D21" s="38"/>
+      <c r="E21" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="19"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="31" t="s">
+      <c r="D22" s="41"/>
+      <c r="E22" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="32"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="19"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="27" t="s">
+      <c r="D23" s="44"/>
+      <c r="E23" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="41"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="19"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="28" t="s">
+      <c r="D24" s="41"/>
+      <c r="E24" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="19"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="46"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="44"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="19"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="19"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="19"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="19"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="19"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="19"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="19"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="19"/>
+      <c r="A36" s="48"/>
       <c r="B36" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="20"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="21"/>
+      <c r="A38" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A2:A37"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" firstPageNumber="0" orientation="landscape" r:id="rId1"/>

</xml_diff>